<commit_message>
Added missing tracks to TrackDataContainer
</commit_message>
<xml_diff>
--- a/SampleData/CircuitJsonData.xlsx
+++ b/SampleData/CircuitJsonData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TaHan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TaHan\Downloads\Codemasters.F1_2020\SampleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CC46E6-E2E0-4E21-8493-48A809A36255}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6090E45F-BFD6-4292-84A5-C8299047E838}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6F558A0A-A852-42E8-B139-D191F1D5A3BC}"/>
+    <workbookView xWindow="6228" yWindow="2352" windowWidth="14448" windowHeight="8916" xr2:uid="{6F558A0A-A852-42E8-B139-D191F1D5A3BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -523,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D8F73D6-063E-49C8-9F06-2821817E03EF}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>